<commit_message>
Rearrange the position (Mohamed)
</commit_message>
<xml_diff>
--- a/Output_data/kappa.xlsx
+++ b/Output_data/kappa.xlsx
@@ -2845,304 +2845,304 @@
         <v>0.01</v>
       </c>
       <c r="CW2">
-        <v>195.3</v>
+        <v>1</v>
       </c>
       <c r="CX2">
-        <v>194.42</v>
+        <v>0.99</v>
       </c>
       <c r="CY2">
-        <v>193.85</v>
+        <v>0.98</v>
       </c>
       <c r="CZ2">
-        <v>193.56</v>
+        <v>0.97</v>
       </c>
       <c r="DA2">
-        <v>193.4</v>
+        <v>0.96</v>
       </c>
       <c r="DB2">
-        <v>192.38</v>
+        <v>0.95</v>
       </c>
       <c r="DC2">
-        <v>191.81</v>
+        <v>0.94</v>
       </c>
       <c r="DD2">
-        <v>189.12</v>
+        <v>0.93</v>
       </c>
       <c r="DE2">
-        <v>189.11</v>
+        <v>0.92</v>
       </c>
       <c r="DF2">
-        <v>187.65</v>
+        <v>0.91</v>
       </c>
       <c r="DG2">
-        <v>186.49</v>
+        <v>0.9</v>
       </c>
       <c r="DH2">
-        <v>186.34</v>
+        <v>0.89</v>
       </c>
       <c r="DI2">
-        <v>185.02</v>
+        <v>0.88</v>
       </c>
       <c r="DJ2">
-        <v>184.67</v>
+        <v>0.87</v>
       </c>
       <c r="DK2">
-        <v>183.95</v>
+        <v>0.86</v>
       </c>
       <c r="DL2">
-        <v>183.54</v>
+        <v>0.85</v>
       </c>
       <c r="DM2">
-        <v>183.36</v>
+        <v>0.84</v>
       </c>
       <c r="DN2">
-        <v>182.25</v>
+        <v>0.83</v>
       </c>
       <c r="DO2">
-        <v>182.02</v>
+        <v>0.82</v>
       </c>
       <c r="DP2">
-        <v>181.02</v>
+        <v>0.81</v>
       </c>
       <c r="DQ2">
-        <v>177.23</v>
+        <v>0.8</v>
       </c>
       <c r="DR2">
-        <v>176.66</v>
+        <v>0.79</v>
       </c>
       <c r="DS2">
-        <v>176.35</v>
+        <v>0.78</v>
       </c>
       <c r="DT2">
-        <v>176.21</v>
+        <v>0.77</v>
       </c>
       <c r="DU2">
-        <v>172.75</v>
+        <v>0.76</v>
       </c>
       <c r="DV2">
-        <v>172.54</v>
+        <v>0.75</v>
       </c>
       <c r="DW2">
-        <v>169.89</v>
+        <v>0.74</v>
       </c>
       <c r="DX2">
-        <v>169.43</v>
+        <v>0.73</v>
       </c>
       <c r="DY2">
-        <v>168.73</v>
+        <v>0.72</v>
       </c>
       <c r="DZ2">
-        <v>168.65</v>
+        <v>0.71</v>
       </c>
       <c r="EA2">
-        <v>167.84</v>
+        <v>0.7</v>
       </c>
       <c r="EB2">
-        <v>166.46</v>
+        <v>0.69</v>
       </c>
       <c r="EC2">
-        <v>164.87</v>
+        <v>0.68</v>
       </c>
       <c r="ED2">
-        <v>163.94</v>
+        <v>0.67</v>
       </c>
       <c r="EE2">
-        <v>162.87</v>
+        <v>0.66</v>
       </c>
       <c r="EF2">
-        <v>162.47</v>
+        <v>0.65</v>
       </c>
       <c r="EG2">
-        <v>161.97</v>
+        <v>0.64</v>
       </c>
       <c r="EH2">
-        <v>161.57</v>
+        <v>0.63</v>
       </c>
       <c r="EI2">
-        <v>160.21</v>
+        <v>0.62</v>
       </c>
       <c r="EJ2">
-        <v>159.01</v>
+        <v>0.61</v>
       </c>
       <c r="EK2">
-        <v>158.51</v>
+        <v>0.6</v>
       </c>
       <c r="EL2">
-        <v>156.03</v>
+        <v>0.59</v>
       </c>
       <c r="EM2">
-        <v>155.19</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="EN2">
-        <v>155.15</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="EO2">
-        <v>155.07</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="EP2">
-        <v>152.30000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="EQ2">
-        <v>151.13999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="ER2">
-        <v>150.65</v>
+        <v>0.53</v>
       </c>
       <c r="ES2">
-        <v>149.71</v>
+        <v>0.52</v>
       </c>
       <c r="ET2">
-        <v>149.19</v>
+        <v>0.51</v>
       </c>
       <c r="EU2">
-        <v>148.02000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="EV2">
-        <v>147.16</v>
+        <v>0.49</v>
       </c>
       <c r="EW2">
-        <v>146.69</v>
+        <v>0.48</v>
       </c>
       <c r="EX2">
-        <v>142.94999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="EY2">
-        <v>142.1</v>
+        <v>0.46</v>
       </c>
       <c r="EZ2">
-        <v>141.72</v>
+        <v>0.45</v>
       </c>
       <c r="FA2">
-        <v>141.61000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="FB2">
-        <v>141.24</v>
+        <v>0.43</v>
       </c>
       <c r="FC2">
-        <v>137.72</v>
+        <v>0.42</v>
       </c>
       <c r="FD2">
-        <v>137.4</v>
+        <v>0.41</v>
       </c>
       <c r="FE2">
-        <v>135.72</v>
+        <v>0.4</v>
       </c>
       <c r="FF2">
-        <v>134.84</v>
+        <v>0.39</v>
       </c>
       <c r="FG2">
-        <v>134.31</v>
+        <v>0.38</v>
       </c>
       <c r="FH2">
-        <v>133.47</v>
+        <v>0.37</v>
       </c>
       <c r="FI2">
-        <v>131.81</v>
+        <v>0.36</v>
       </c>
       <c r="FJ2">
-        <v>129.77000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="FK2">
-        <v>128.16</v>
+        <v>0.34</v>
       </c>
       <c r="FL2">
-        <v>127.26</v>
+        <v>0.33</v>
       </c>
       <c r="FM2">
-        <v>126.56</v>
+        <v>0.32</v>
       </c>
       <c r="FN2">
-        <v>126.34</v>
+        <v>0.31</v>
       </c>
       <c r="FO2">
-        <v>123.32</v>
+        <v>0.3</v>
       </c>
       <c r="FP2">
-        <v>122.27</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="FQ2">
-        <v>121.48</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="FR2">
-        <v>119.56</v>
+        <v>0.27</v>
       </c>
       <c r="FS2">
-        <v>119.46</v>
+        <v>0.26</v>
       </c>
       <c r="FT2">
-        <v>119.03</v>
+        <v>0.25</v>
       </c>
       <c r="FU2">
-        <v>117.85</v>
+        <v>0.24</v>
       </c>
       <c r="FV2">
-        <v>116.23</v>
+        <v>0.23</v>
       </c>
       <c r="FW2">
-        <v>115.02</v>
+        <v>0.22</v>
       </c>
       <c r="FX2">
-        <v>112.74</v>
+        <v>0.21</v>
       </c>
       <c r="FY2">
-        <v>110.32</v>
+        <v>0.2</v>
       </c>
       <c r="FZ2">
-        <v>109.99</v>
+        <v>0.19</v>
       </c>
       <c r="GA2">
-        <v>107.9</v>
+        <v>0.18</v>
       </c>
       <c r="GB2">
-        <v>106.1</v>
+        <v>0.17</v>
       </c>
       <c r="GC2">
-        <v>105.17</v>
+        <v>0.16</v>
       </c>
       <c r="GD2">
-        <v>104.76</v>
+        <v>0.15</v>
       </c>
       <c r="GE2">
-        <v>103.5</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="GF2">
-        <v>103.08</v>
+        <v>0.13</v>
       </c>
       <c r="GG2">
-        <v>102.37</v>
+        <v>0.12</v>
       </c>
       <c r="GH2">
-        <v>100.05</v>
+        <v>0.11</v>
       </c>
       <c r="GI2">
-        <v>97.75</v>
+        <v>0.1</v>
       </c>
       <c r="GJ2">
-        <v>97.38</v>
+        <v>0.09</v>
       </c>
       <c r="GK2">
-        <v>93.53</v>
+        <v>0.08</v>
       </c>
       <c r="GL2">
-        <v>93.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="GM2">
-        <v>90.83</v>
+        <v>0.06</v>
       </c>
       <c r="GN2">
-        <v>89.28</v>
+        <v>0.05</v>
       </c>
       <c r="GO2">
-        <v>88.8</v>
+        <v>0.04</v>
       </c>
       <c r="GP2">
-        <v>87.53</v>
+        <v>0.03</v>
       </c>
       <c r="GQ2">
-        <v>86.18</v>
+        <v>0.02</v>
       </c>
       <c r="GR2">
-        <v>86.09</v>
+        <v>0.01</v>
       </c>
       <c r="GS2">
         <v>84.11</v>

</xml_diff>